<commit_message>
report t session 19/12/24
</commit_message>
<xml_diff>
--- a/task/training_session_monitoring.xlsx
+++ b/task/training_session_monitoring.xlsx
@@ -8,18 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ad0791/Desktop/Hanwash.mwater.dev/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{296EC62F-3653-C441-A7B5-747D7891A2AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C8BEB7-AA17-E247-9FB0-795E66169D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="540" windowWidth="25040" windowHeight="14860" xr2:uid="{31B2DF59-D489-1B42-A6C4-E1B1C858A295}"/>
   </bookViews>
   <sheets>
-    <sheet name="project_teams" sheetId="1" r:id="rId1"/>
-    <sheet name="mayors" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
+    <sheet name="project_teams" sheetId="1" r:id="rId2"/>
+    <sheet name="mayors" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">project_teams!$A$1:$J$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">project_teams!$A$1:$J$15</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
+  <pivotCaches>
+    <pivotCache cacheId="3" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="97">
   <si>
     <t>zone</t>
   </si>
@@ -297,13 +301,47 @@
   </si>
   <si>
     <t>(YES)</t>
+  </si>
+  <si>
+    <t>Count of zone</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>(blank)</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>haitian group</t>
+  </si>
+  <si>
+    <t>volunteers group</t>
+  </si>
+  <si>
+    <t>trained</t>
+  </si>
+  <si>
+    <t>not trained</t>
+  </si>
+  <si>
+    <t>status/group</t>
+  </si>
+  <si>
+    <t>Training session / Project teams 
+for the month of December 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -339,8 +377,29 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +421,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC8C1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -414,6 +491,23 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -421,6 +515,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC8C1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -430,6 +529,300 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Microsoft Office User" refreshedDate="45645.545760879628" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="14" xr:uid="{747E659F-9059-ED43-9196-548F0CF5A3DC}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:J15" sheet="project_teams"/>
+  </cacheSource>
+  <cacheFields count="10">
+    <cacheField name="zone" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="nom et prenom" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="#tel" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="email" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="has_mwater_acc" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="uname" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="upass" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="english" numFmtId="0">
+      <sharedItems count="2">
+        <s v="no"/>
+        <s v="yes"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="CPE's training" numFmtId="0">
+      <sharedItems containsBlank="1" count="2">
+        <s v="YES"/>
+        <m/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="CAP training" numFmtId="0">
+      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="14">
+  <r>
+    <s v="Cavaillon"/>
+    <s v="Emmanuel Charles"/>
+    <s v="+509 48 13 7815"/>
+    <s v="emmanuelcharle23@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Cavaillon"/>
+    <s v="Sandra Hemstead"/>
+    <m/>
+    <s v="sandrahemstead@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Leogane"/>
+    <s v="Bob Chagrasulis"/>
+    <m/>
+    <s v="bobchagrasulis@aol.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Leogane"/>
+    <s v="Dan Balfe"/>
+    <m/>
+    <s v="danbalferotary@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Leogane"/>
+    <s v="Jean Marc BRISSAU"/>
+    <m/>
+    <s v="jmbrissau@gmail.com"/>
+    <s v="YES"/>
+    <s v="jean.marie.brissau"/>
+    <s v="Hanwash1234"/>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Terre Neuve"/>
+    <s v="Covington Cynde"/>
+    <m/>
+    <s v="cyndecovington@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Terre Neuve"/>
+    <s v="Ron Denham"/>
+    <m/>
+    <s v="ron.denham1021@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Terre Neuve"/>
+    <s v="Tom Schmidt"/>
+    <m/>
+    <s v="tomschmidt1516@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Terre Neuve"/>
+    <s v="Jill Duerig"/>
+    <m/>
+    <s v="jillduerig@hotmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Ferrier"/>
+    <s v="Sherry Chamberlain"/>
+    <m/>
+    <s v="sherry@adobie.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Ferrier"/>
+    <s v="Magarette Georges"/>
+    <s v="+509 37 30 3326"/>
+    <s v="magarettegeorges@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Pignon"/>
+    <s v="Moussanto Dantil"/>
+    <s v="509 3628 4962"/>
+    <s v="dantilplus@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="0"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Pignon"/>
+    <s v="Jan Pooley"/>
+    <m/>
+    <s v="jpooley5@cox.net"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="0"/>
+    <m/>
+  </r>
+  <r>
+    <s v="Pignon"/>
+    <s v="Christine Isham"/>
+    <m/>
+    <s v="crisdanish@gmail.com"/>
+    <s v="YES"/>
+    <m/>
+    <m/>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{4CD7A304-F613-CF4C-87B0-D565A918A685}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="8"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="7"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of zone" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -728,11 +1121,172 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4341B1E5-7FE3-0641-8785-6D62AB3B48B1}">
+  <dimension ref="A3:K18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:11">
+      <c r="A3" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="15">
+        <v>3</v>
+      </c>
+      <c r="C5" s="15">
+        <v>6</v>
+      </c>
+      <c r="D5" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="15">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
+        <v>4</v>
+      </c>
+      <c r="D6" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="15">
+        <v>4</v>
+      </c>
+      <c r="C7" s="15">
+        <v>10</v>
+      </c>
+      <c r="D7" s="15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="H13" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" ht="37" customHeight="1">
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="20"/>
+    </row>
+    <row r="15" spans="1:11" ht="21">
+      <c r="H15" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="I15" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="K15" s="21" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="21">
+      <c r="H16" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="18">
+        <v>3</v>
+      </c>
+      <c r="J16" s="18">
+        <v>6</v>
+      </c>
+      <c r="K16" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="8:11" ht="21">
+      <c r="H17" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="I17" s="18">
+        <v>1</v>
+      </c>
+      <c r="J17" s="18">
+        <v>4</v>
+      </c>
+      <c r="K17" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="8:11" ht="21">
+      <c r="H18" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="18">
+        <v>4</v>
+      </c>
+      <c r="J18" s="18">
+        <v>10</v>
+      </c>
+      <c r="K18" s="24">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H13:K14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C36F2941-11D6-6F43-B65B-628189CF42E4}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -801,7 +1355,9 @@
       <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10">
@@ -1037,7 +1593,9 @@
       <c r="H12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
@@ -1061,7 +1619,9 @@
       <c r="H13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
@@ -1123,7 +1683,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E715955F-24F3-D846-AC9C-70C2FEE042AD}">
   <dimension ref="A1:H7"/>
   <sheetViews>

</xml_diff>